<commit_message>
Use existing rg and dnsZone (broken ingress)
</commit_message>
<xml_diff>
--- a/resource_calculations.xlsx
+++ b/resource_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin.mitchinson/repos/urbanos/hercules/juno/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD60DBEE-2E26-8A4D-8D0E-7946244A5FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E3B1BC-5781-4C41-8463-10A07788F003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20680" xr2:uid="{9721AC37-4263-8A4E-A5EF-CE47FC21A0CD}"/>
+    <workbookView xWindow="17900" yWindow="500" windowWidth="17920" windowHeight="20680" xr2:uid="{9721AC37-4263-8A4E-A5EF-CE47FC21A0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -268,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -278,9 +278,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D200D8-F694-E04F-BC62-04F76460BF37}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -611,68 +608,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="9">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>2000</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3">
         <v>16</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3">
         <v>8000</v>
       </c>
-      <c r="E3" s="9">
-        <v>0</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>8.3199999999999996E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4">
         <v>2000</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4">
         <v>8</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4">
         <v>4000</v>
       </c>
-      <c r="E4" s="9">
-        <v>9</v>
-      </c>
-      <c r="F4" s="9">
+      <c r="E4">
+        <v>11</v>
+      </c>
+      <c r="F4">
         <v>4.1599999999999998E-2</v>
       </c>
     </row>
@@ -692,7 +680,7 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5">
         <v>0.16600000000000001</v>
       </c>
     </row>
@@ -715,10 +703,10 @@
       <c r="A14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14">
         <v>1000</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" s="5">
@@ -729,10 +717,10 @@
       <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15">
         <v>250</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" s="5">
@@ -743,10 +731,10 @@
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16">
         <v>300</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" s="5">
@@ -757,10 +745,10 @@
       <c r="A17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17">
         <v>400</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" s="5">
@@ -771,10 +759,10 @@
       <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18">
         <v>250</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" s="5">
@@ -785,10 +773,10 @@
       <c r="A19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19">
         <v>250</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" s="5">
@@ -799,10 +787,10 @@
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20">
         <v>250</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20">
         <v>0</v>
       </c>
       <c r="D20" s="5">
@@ -813,10 +801,10 @@
       <c r="A21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21">
         <v>400</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" s="5">
@@ -825,30 +813,24 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="9">
-        <v>500</v>
-      </c>
-      <c r="C25" s="9">
+      <c r="B25">
+        <v>500</v>
+      </c>
+      <c r="C25">
         <v>0.5</v>
       </c>
       <c r="D25" s="5">
@@ -859,10 +841,10 @@
       <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="9">
-        <v>500</v>
-      </c>
-      <c r="C26" s="9">
+      <c r="B26">
+        <v>500</v>
+      </c>
+      <c r="C26">
         <v>0</v>
       </c>
       <c r="D26" s="5">
@@ -873,10 +855,10 @@
       <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27">
         <v>200</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27">
         <v>0</v>
       </c>
       <c r="D27" s="5">
@@ -887,10 +869,10 @@
       <c r="A28" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="9">
-        <v>500</v>
-      </c>
-      <c r="C28" s="9">
+      <c r="B28">
+        <v>500</v>
+      </c>
+      <c r="C28">
         <v>4</v>
       </c>
       <c r="D28" s="5">
@@ -901,10 +883,10 @@
       <c r="A29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29">
         <v>200</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29">
         <v>0.5</v>
       </c>
       <c r="D29" s="5">
@@ -915,10 +897,10 @@
       <c r="A30" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30">
         <v>300</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30">
         <v>4</v>
       </c>
       <c r="D30" s="5">
@@ -929,10 +911,10 @@
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31">
         <v>800</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31">
         <v>0</v>
       </c>
       <c r="D31" s="5">
@@ -943,10 +925,10 @@
       <c r="A32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32">
         <v>800</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32">
         <v>0</v>
       </c>
       <c r="D32" s="5">
@@ -957,10 +939,10 @@
       <c r="A33" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="9">
-        <v>500</v>
-      </c>
-      <c r="C33" s="9">
+      <c r="B33">
+        <v>500</v>
+      </c>
+      <c r="C33">
         <v>0</v>
       </c>
       <c r="D33" s="5">
@@ -971,10 +953,10 @@
       <c r="A34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34">
         <v>250</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34">
         <v>1</v>
       </c>
       <c r="D34" s="5">
@@ -985,36 +967,27 @@
       <c r="A35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39">
         <v>3000</v>
       </c>
-      <c r="C39" s="9"/>
       <c r="D39" s="5">
         <v>2500</v>
       </c>
@@ -1024,8 +997,6 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
       <c r="D40" s="5"/>
       <c r="E40" t="s">
         <v>36</v>
@@ -1035,10 +1006,9 @@
       <c r="A41" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41">
         <v>400</v>
       </c>
-      <c r="C41" s="9"/>
       <c r="D41" s="5">
         <v>500</v>
       </c>
@@ -1056,83 +1026,75 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="9" t="s">
+      <c r="A45" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45">
         <f>(B4*E4)+(B3*E3)+(B5*E5)</f>
-        <v>18000</v>
-      </c>
-      <c r="C45" s="9">
+        <v>22000</v>
+      </c>
+      <c r="C45">
         <f>(C4*E4)+(C3*E3)+(C5*E5)</f>
-        <v>72</v>
-      </c>
-      <c r="D45" s="9">
+        <v>88</v>
+      </c>
+      <c r="D45">
         <f>(D4*E4)+(D3*E3)+(D5+E5)</f>
-        <v>52000</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="9" t="s">
+      <c r="A46" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46">
         <f>B45-SUM(B13:B42)</f>
-        <v>6400</v>
-      </c>
-      <c r="C46" s="9">
+        <v>10400</v>
+      </c>
+      <c r="C46">
         <f>C45-SUM(C13:C42)</f>
-        <v>60</v>
-      </c>
-      <c r="D46" s="9">
+        <v>76</v>
+      </c>
+      <c r="D46">
         <f>D45-SUM(D13:D42)</f>
-        <v>33350</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-    </row>
+        <v>41350</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B48" s="2">
         <f>(E3*F3)+(E4*F4)+(E5*F5)</f>
-        <v>0.37439999999999996</v>
+        <v>0.45760000000000001</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B49">
         <v>5</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B51" s="9">
+      <c r="B51">
         <f>(B48+B49*C49)</f>
-        <v>0.49939999999999996</v>
-      </c>
-      <c r="C51" s="9"/>
+        <v>0.58260000000000001</v>
+      </c>
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1141,7 +1103,7 @@
       </c>
       <c r="B52" s="7">
         <f>B51*732</f>
-        <v>365.56079999999997</v>
+        <v>426.46320000000003</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="8"/>

</xml_diff>

<commit_message>
demo-urbanos.com + correct node pools w persistence affinity
</commit_message>
<xml_diff>
--- a/resource_calculations.xlsx
+++ b/resource_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin.mitchinson/repos/urbanos/hercules/juno/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E3B1BC-5781-4C41-8463-10A07788F003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EF79DF-1804-A944-A226-C4A3B473FD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17900" yWindow="500" windowWidth="17920" windowHeight="20680" xr2:uid="{9721AC37-4263-8A4E-A5EF-CE47FC21A0CD}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="19900" xr2:uid="{9721AC37-4263-8A4E-A5EF-CE47FC21A0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Standard_B2ms</t>
   </si>
@@ -50,9 +50,6 @@
     <t>CPU (m)</t>
   </si>
   <si>
-    <t>RAM (M)</t>
-  </si>
-  <si>
     <t>Amount in Pool</t>
   </si>
   <si>
@@ -149,10 +146,25 @@
     <t>kube-system estimate seems wrong, limit is 5x higher</t>
   </si>
   <si>
-    <t>Certs? Not in yaml?</t>
-  </si>
-  <si>
     <t>Standard_B4ms</t>
+  </si>
+  <si>
+    <t>2vCPU -&gt; 1900m alo</t>
+  </si>
+  <si>
+    <t>RAM (GiB)</t>
+  </si>
+  <si>
+    <t>Certs? Not in yaml</t>
+  </si>
+  <si>
+    <t>4000M RAM -&gt; 2200 (persistence VMs (3) need 3000, so no B2s nodes are eligible</t>
+  </si>
+  <si>
+    <t>node affin high ram</t>
+  </si>
+  <si>
+    <t>8000M -&gt; 5364</t>
   </si>
 </sst>
 </file>
@@ -592,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D200D8-F694-E04F-BC62-04F76460BF37}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,10 +616,13 @@
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -615,58 +630,70 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>2000</v>
+        <v>1900</v>
       </c>
       <c r="C3">
         <v>16</v>
       </c>
       <c r="D3">
-        <v>8000</v>
+        <v>5364</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <v>8.3199999999999996E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>2000</v>
+        <v>1900</v>
       </c>
       <c r="C4">
         <v>8</v>
       </c>
       <c r="D4">
-        <v>4000</v>
+        <v>2200</v>
       </c>
       <c r="E4">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F4">
         <v>4.1599999999999998E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>4000</v>
@@ -684,10 +711,10 @@
         <v>0.16600000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="2">
         <v>150</v>
@@ -699,9 +726,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14">
         <v>1000</v>
@@ -713,9 +740,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>250</v>
@@ -727,9 +754,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>300</v>
@@ -741,9 +768,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17">
         <v>400</v>
@@ -755,9 +782,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>250</v>
@@ -769,9 +796,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <v>250</v>
@@ -783,9 +810,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>250</v>
@@ -797,9 +824,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21">
         <v>400</v>
@@ -811,35 +838,35 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25">
         <v>500</v>
       </c>
       <c r="C25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D25" s="5">
         <v>1500</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26">
         <v>500</v>
@@ -851,23 +878,23 @@
         <v>400</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27">
         <v>200</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28">
         <v>500</v>
@@ -879,9 +906,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29">
         <v>200</v>
@@ -893,9 +920,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30">
         <v>300</v>
@@ -907,9 +934,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31">
         <v>800</v>
@@ -920,10 +947,13 @@
       <c r="D31" s="5">
         <v>3000</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32">
         <v>800</v>
@@ -934,10 +964,13 @@
       <c r="D32" s="5">
         <v>3000</v>
       </c>
+      <c r="E32" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33">
         <v>500</v>
@@ -951,7 +984,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34">
         <v>250</v>
@@ -965,7 +998,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D35" s="5"/>
     </row>
@@ -983,7 +1016,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B39">
         <v>3000</v>
@@ -992,19 +1025,19 @@
         <v>2500</v>
       </c>
       <c r="E39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="D40" s="5"/>
       <c r="E40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41">
         <v>400</v>
@@ -1015,7 +1048,7 @@
     </row>
     <row r="42" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="7">
         <v>400</v>
@@ -1027,11 +1060,11 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B45">
         <f>(B4*E4)+(B3*E3)+(B5*E5)</f>
-        <v>22000</v>
+        <v>15200</v>
       </c>
       <c r="C45">
         <f>(C4*E4)+(C3*E3)+(C5*E5)</f>
@@ -1039,30 +1072,30 @@
       </c>
       <c r="D45">
         <f>(D4*E4)+(D3*E3)+(D5+E5)</f>
-        <v>60000</v>
+        <v>43092</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46">
         <f>B45-SUM(B13:B42)</f>
-        <v>10400</v>
+        <v>3600</v>
       </c>
       <c r="C46">
         <f>C45-SUM(C13:C42)</f>
-        <v>76</v>
+        <v>74.5</v>
       </c>
       <c r="D46">
         <f>D45-SUM(D13:D42)</f>
-        <v>41350</v>
+        <v>24442</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B48" s="2">
         <f>(E3*F3)+(E4*F4)+(E5*F5)</f>
@@ -1073,7 +1106,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B49">
         <v>5</v>
@@ -1089,7 +1122,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B51">
         <f>(B48+B49*C49)</f>
@@ -1099,7 +1132,7 @@
     </row>
     <row r="52" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B52" s="7">
         <f>B51*732</f>

</xml_diff>

<commit_message>
Readme and resource updates
</commit_message>
<xml_diff>
--- a/resource_calculations.xlsx
+++ b/resource_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin.mitchinson/repos/urbanos/hercules/juno/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EF79DF-1804-A944-A226-C4A3B473FD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A107BB2-46D8-DC4D-96A3-C0B61BBC799F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="19900" xr2:uid="{9721AC37-4263-8A4E-A5EF-CE47FC21A0CD}"/>
   </bookViews>
@@ -653,7 +653,7 @@
         <v>5364</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>8.3199999999999996E-2</v>
@@ -705,7 +705,7 @@
         <v>16000</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0.16600000000000001</v>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="B45">
         <f>(B4*E4)+(B3*E3)+(B5*E5)</f>
-        <v>15200</v>
+        <v>15400</v>
       </c>
       <c r="C45">
         <f>(C4*E4)+(C3*E3)+(C5*E5)</f>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="D45">
         <f>(D4*E4)+(D3*E3)+(D5+E5)</f>
-        <v>43092</v>
+        <v>32365</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="B46">
         <f>B45-SUM(B13:B42)</f>
-        <v>3600</v>
+        <v>3800</v>
       </c>
       <c r="C46">
         <f>C45-SUM(C13:C42)</f>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="D46">
         <f>D45-SUM(D13:D42)</f>
-        <v>24442</v>
+        <v>13715</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1099,7 +1099,7 @@
       </c>
       <c r="B48" s="2">
         <f>(E3*F3)+(E4*F4)+(E5*F5)</f>
-        <v>0.45760000000000001</v>
+        <v>0.45720000000000005</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="B51">
         <f>(B48+B49*C49)</f>
-        <v>0.58260000000000001</v>
+        <v>0.58220000000000005</v>
       </c>
       <c r="D51" s="5"/>
     </row>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B52" s="7">
         <f>B51*732</f>
-        <v>426.46320000000003</v>
+        <v>426.17040000000003</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="8"/>

</xml_diff>